<commit_message>
Fix branch instruction format
</commit_message>
<xml_diff>
--- a/RegisterDesign.xlsx
+++ b/RegisterDesign.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\cs1\2020\jbattista20\CS-401-1-CompArch\FinalProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\cs1\2020\jbattista20\CS-401-1-CompArch\FinalProject\MP_1_Compiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="84">
   <si>
     <t>Stack Pointer</t>
   </si>
@@ -153,12 +153,6 @@
     <t>Source Register 2</t>
   </si>
   <si>
-    <t>beqi</t>
-  </si>
-  <si>
-    <t>bnei</t>
-  </si>
-  <si>
     <t>Loop Counter value</t>
   </si>
   <si>
@@ -267,13 +261,22 @@
     <t>01000000</t>
   </si>
   <si>
-    <t>11000001</t>
-  </si>
-  <si>
     <t>00010000</t>
   </si>
   <si>
     <t>00100000</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Flags</t>
+  </si>
+  <si>
+    <t>$flg</t>
+  </si>
+  <si>
+    <t>Not directly modifiable by programmer</t>
   </si>
 </sst>
 </file>
@@ -619,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,6 +741,20 @@
         <v>16</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -746,10 +763,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,12 +794,12 @@
         <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -800,16 +817,16 @@
         <v>0</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -827,16 +844,16 @@
         <v>1</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J4" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L4" t="s">
         <v>56</v>
-      </c>
-      <c r="K4" t="s">
-        <v>54</v>
-      </c>
-      <c r="L4" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -857,13 +874,13 @@
       </c>
       <c r="F5" s="5"/>
       <c r="J5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -894,11 +911,11 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F8" s="5"/>
       <c r="J8" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K8" s="2">
         <v>0</v>
@@ -940,10 +957,10 @@
         <v>0</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -964,10 +981,10 @@
         <v>1</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -991,7 +1008,7 @@
       </c>
       <c r="F11" s="5"/>
       <c r="J11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -1015,7 +1032,7 @@
       </c>
       <c r="F12" s="5"/>
       <c r="J12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L12">
         <v>1</v>
@@ -1023,23 +1040,23 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3">
         <v>4</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M13">
         <v>1</v>
@@ -1047,23 +1064,23 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3">
         <v>5</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -1074,17 +1091,17 @@
         <v>32</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3">
         <v>6</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -1097,7 +1114,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F17" s="5"/>
     </row>
@@ -1106,147 +1123,109 @@
         <v>27</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3">
         <v>0</v>
       </c>
       <c r="F18" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3">
+        <v>0</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3">
-        <v>1</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20">
-        <v>2</v>
-      </c>
-      <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21">
-        <v>3</v>
-      </c>
-      <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F22" s="5"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3">
-        <v>0</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" t="s">
-        <v>25</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25" s="5"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" t="s">
-        <v>25</v>
-      </c>
-      <c r="E26">
-        <v>2</v>
-      </c>
-      <c r="F26" s="5"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F27" s="5"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F28" s="5"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3">
-        <v>0</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update opcodes in RegisterDesign
Now includes opcodes for list operations
Update existing opcodes in assembler
Still need to add new opcodes to assembler
</commit_message>
<xml_diff>
--- a/RegisterDesign.xlsx
+++ b/RegisterDesign.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\cs1\2020\jbattista20\CS-401-1-CompArch\FinalProject\MP_1_Compiler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CS-401-1-CompArch\FinalProject\MP_1_Compiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="96">
   <si>
     <t>Stack Pointer</t>
   </si>
@@ -159,12 +159,6 @@
     <t>Ladd</t>
   </si>
   <si>
-    <t>Lsum</t>
-  </si>
-  <si>
-    <t>Lalu</t>
-  </si>
-  <si>
     <t>lw</t>
   </si>
   <si>
@@ -261,9 +255,6 @@
     <t>01000000</t>
   </si>
   <si>
-    <t>00010000</t>
-  </si>
-  <si>
     <t>00100000</t>
   </si>
   <si>
@@ -277,6 +268,51 @@
   </si>
   <si>
     <t>Not directly modifiable by programmer</t>
+  </si>
+  <si>
+    <t>00010001</t>
+  </si>
+  <si>
+    <t>LLoad</t>
+  </si>
+  <si>
+    <t>LStore</t>
+  </si>
+  <si>
+    <t>Source Register</t>
+  </si>
+  <si>
+    <t>Destination Register</t>
+  </si>
+  <si>
+    <t>10010010</t>
+  </si>
+  <si>
+    <t>Land</t>
+  </si>
+  <si>
+    <t>10010011</t>
+  </si>
+  <si>
+    <t>00010100</t>
+  </si>
+  <si>
+    <t>Lor</t>
+  </si>
+  <si>
+    <t>Lxor</t>
+  </si>
+  <si>
+    <t>00010101</t>
+  </si>
+  <si>
+    <t>00010110</t>
+  </si>
+  <si>
+    <t>Lnot</t>
+  </si>
+  <si>
+    <t>00010111</t>
   </si>
 </sst>
 </file>
@@ -624,7 +660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -743,16 +779,16 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -763,10 +799,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R27"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,12 +830,12 @@
         <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -817,16 +853,16 @@
         <v>0</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -844,16 +880,16 @@
         <v>1</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" t="s">
         <v>54</v>
-      </c>
-      <c r="K4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L4" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -874,13 +910,13 @@
       </c>
       <c r="F5" s="5"/>
       <c r="J5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -911,11 +947,11 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F8" s="5"/>
       <c r="J8" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K8" s="2">
         <v>0</v>
@@ -957,10 +993,10 @@
         <v>0</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -981,10 +1017,10 @@
         <v>1</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -1008,7 +1044,7 @@
       </c>
       <c r="F11" s="5"/>
       <c r="J11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -1032,7 +1068,7 @@
       </c>
       <c r="F12" s="5"/>
       <c r="J12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L12">
         <v>1</v>
@@ -1040,23 +1076,23 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3">
         <v>4</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M13">
         <v>1</v>
@@ -1064,23 +1100,23 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3">
         <v>5</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -1091,7 +1127,7 @@
         <v>32</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>42</v>
@@ -1101,7 +1137,7 @@
         <v>6</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -1114,7 +1150,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F17" s="5"/>
     </row>
@@ -1123,7 +1159,7 @@
         <v>27</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1131,7 +1167,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1157,75 +1193,161 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="1"/>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3">
-        <v>0</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23" s="5"/>
+      <c r="B23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3">
+        <v>1</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" t="s">
-        <v>25</v>
+        <v>82</v>
+      </c>
+      <c r="B24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" t="s">
+        <v>48</v>
       </c>
       <c r="E24">
         <v>2</v>
       </c>
-      <c r="F24" s="5"/>
+      <c r="F24" s="5" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F25" s="5"/>
+      <c r="A25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F26" s="5"/>
+      <c r="A26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3">
+      <c r="A27" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27">
+        <v>5</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28">
+        <v>6</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29">
+        <v>7</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3">
         <v>0</v>
       </c>
-      <c r="F27" s="5" t="s">
-        <v>79</v>
+      <c r="F33" s="5" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add list commands to parser and spreadsheet
Add Ladd, LL, and LS to the parser
Add three list registers to the parser
</commit_message>
<xml_diff>
--- a/RegisterDesign.xlsx
+++ b/RegisterDesign.xlsx
@@ -802,7 +802,7 @@
   <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,16 +1223,17 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E24">
+      <c r="D24" s="3"/>
+      <c r="E24" s="3">
         <v>2</v>
       </c>
       <c r="F24" s="5" t="s">
@@ -1240,16 +1241,17 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E25">
+      <c r="D25" s="3"/>
+      <c r="E25" s="3">
         <v>3</v>
       </c>
       <c r="F25" s="5" t="s">

</xml_diff>

<commit_message>
Added control unit file, created inputs and outputs.
ALU connection completed, but need to implement Load List, and Store
List, and connect to RAM.
TODO: Implement connection to RAM, and connect to main ALU/control unit.
</commit_message>
<xml_diff>
--- a/RegisterDesign.xlsx
+++ b/RegisterDesign.xlsx
@@ -801,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
The control unit is working!
</commit_message>
<xml_diff>
--- a/RegisterDesign.xlsx
+++ b/RegisterDesign.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="121">
   <si>
     <t>Stack Pointer</t>
   </si>
@@ -386,6 +386,9 @@
   </si>
   <si>
     <t>If this doesn't work, then we can just implement sequential lw and sw commands in the compiler.</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -1437,13 +1440,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="L10" sqref="B10:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="7" max="10" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
@@ -1503,9 +1512,15 @@
       <c r="G2" s="6">
         <v>0</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="H2" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J2" s="6">
+        <v>1</v>
+      </c>
       <c r="K2" s="6"/>
       <c r="L2" s="6" t="s">
         <v>106</v>
@@ -1533,9 +1548,15 @@
       <c r="G3" s="6">
         <v>0</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
+      <c r="H3" s="6">
+        <v>0</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0</v>
+      </c>
       <c r="K3" s="6"/>
       <c r="L3" s="6" t="s">
         <v>107</v>
@@ -1563,41 +1584,53 @@
       <c r="G4" s="6">
         <v>0</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
+      <c r="H4" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0</v>
+      </c>
       <c r="K4" s="6"/>
       <c r="L4" s="6" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="6">
-        <v>1</v>
-      </c>
-      <c r="C5" s="6">
-        <v>1</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6" t="s">
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1618,14 +1651,20 @@
         <v>0</v>
       </c>
       <c r="F6" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="6">
         <v>0</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
+      <c r="H6" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0</v>
+      </c>
       <c r="K6" s="6"/>
       <c r="L6" s="6" t="s">
         <v>44</v>
@@ -1648,14 +1687,20 @@
         <v>1</v>
       </c>
       <c r="F7" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="6">
         <v>0</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
+      <c r="H7" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0</v>
+      </c>
       <c r="K7" s="6"/>
       <c r="L7" s="6" t="s">
         <v>45</v>
@@ -1703,9 +1748,15 @@
       <c r="G9" s="6">
         <v>0</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
+      <c r="H9" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J9" s="6">
+        <v>0</v>
+      </c>
       <c r="K9" s="6"/>
       <c r="L9" s="6" t="s">
         <v>27</v>
@@ -1733,9 +1784,15 @@
       <c r="G10" s="6">
         <v>0</v>
       </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
+      <c r="H10" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0</v>
+      </c>
       <c r="K10" s="6"/>
       <c r="L10" s="6" t="s">
         <v>111</v>
@@ -1763,9 +1820,15 @@
       <c r="G11" s="6">
         <v>0</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
+      <c r="H11" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J11" s="6">
+        <v>0</v>
+      </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6" t="s">
         <v>112</v>
@@ -1793,9 +1856,15 @@
       <c r="G12" s="6">
         <v>0</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
+      <c r="H12" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J12" s="6">
+        <v>0</v>
+      </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6" t="s">
         <v>113</v>
@@ -1823,9 +1892,15 @@
       <c r="G13" s="6">
         <v>1</v>
       </c>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
+      <c r="H13" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J13" s="6">
+        <v>0</v>
+      </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6" t="s">
         <v>61</v>
@@ -1847,29 +1922,409 @@
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="6">
+        <v>1</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0</v>
+      </c>
+      <c r="E23" s="6">
+        <v>0</v>
+      </c>
+      <c r="F23" s="6">
+        <v>0</v>
+      </c>
+      <c r="G23" s="6">
+        <v>0</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J23" s="6">
+        <v>1</v>
+      </c>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="6">
+        <v>1</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0</v>
+      </c>
+      <c r="E24" s="6">
+        <v>0</v>
+      </c>
+      <c r="F24" s="6">
+        <v>0</v>
+      </c>
+      <c r="G24" s="6">
+        <v>0</v>
+      </c>
+      <c r="H24" s="6">
+        <v>0</v>
+      </c>
+      <c r="I24" s="6">
+        <v>0</v>
+      </c>
+      <c r="J24" s="6">
+        <v>0</v>
+      </c>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="6">
+        <v>1</v>
+      </c>
+      <c r="C25" s="6">
+        <v>1</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0</v>
+      </c>
+      <c r="E25" s="6">
+        <v>0</v>
+      </c>
+      <c r="F25" s="6">
+        <v>0</v>
+      </c>
+      <c r="G25" s="6">
+        <v>0</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J25" s="6">
+        <v>0</v>
+      </c>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="7">
+        <v>1</v>
+      </c>
+      <c r="C26" s="7">
+        <v>1</v>
+      </c>
+      <c r="D26" s="7">
+        <v>0</v>
+      </c>
+      <c r="E26" s="7">
+        <v>0</v>
+      </c>
+      <c r="F26" s="7">
+        <v>0</v>
+      </c>
+      <c r="G26" s="7">
+        <v>0</v>
+      </c>
+      <c r="H26" s="7">
+        <v>0</v>
+      </c>
+      <c r="I26" s="7">
+        <v>0</v>
+      </c>
+      <c r="J26" s="7">
+        <v>0</v>
+      </c>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="6">
+        <v>1</v>
+      </c>
+      <c r="C27" s="6">
+        <v>1</v>
+      </c>
+      <c r="D27" s="6">
+        <v>0</v>
+      </c>
+      <c r="E27" s="6">
+        <v>0</v>
+      </c>
+      <c r="F27" s="6">
+        <v>1</v>
+      </c>
+      <c r="G27" s="6">
+        <v>0</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J27" s="6">
+        <v>0</v>
+      </c>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="6">
+        <v>0</v>
+      </c>
+      <c r="C28" s="6">
+        <v>1</v>
+      </c>
+      <c r="D28" s="6">
+        <v>0</v>
+      </c>
+      <c r="E28" s="6">
+        <v>1</v>
+      </c>
+      <c r="F28" s="6">
+        <v>0</v>
+      </c>
+      <c r="G28" s="6">
+        <v>0</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J28" s="6">
+        <v>0</v>
+      </c>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="7">
+        <v>0</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="6">
+        <v>0</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30" s="6">
+        <v>1</v>
+      </c>
+      <c r="E30" s="6">
+        <v>0</v>
+      </c>
+      <c r="F30" s="6">
+        <v>0</v>
+      </c>
+      <c r="G30" s="6">
+        <v>0</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J30" s="6">
+        <v>0</v>
+      </c>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="6">
+        <v>0</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" s="6">
+        <v>0</v>
+      </c>
+      <c r="E31" s="6">
+        <v>0</v>
+      </c>
+      <c r="F31" s="6">
+        <v>0</v>
+      </c>
+      <c r="G31" s="6">
+        <v>0</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J31" s="6">
+        <v>0</v>
+      </c>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="6">
+        <v>0</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D32" s="6">
+        <v>0</v>
+      </c>
+      <c r="E32" s="6">
+        <v>0</v>
+      </c>
+      <c r="F32" s="6">
+        <v>0</v>
+      </c>
+      <c r="G32" s="6">
+        <v>0</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J32" s="6">
+        <v>0</v>
+      </c>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B33" s="6">
+        <v>0</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" s="6">
+        <v>0</v>
+      </c>
+      <c r="E33" s="6">
+        <v>0</v>
+      </c>
+      <c r="F33" s="6">
+        <v>0</v>
+      </c>
+      <c r="G33" s="6">
+        <v>0</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J33" s="6">
+        <v>0</v>
+      </c>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="6">
+        <v>0</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D34" s="6">
+        <v>0</v>
+      </c>
+      <c r="E34" s="6">
+        <v>0</v>
+      </c>
+      <c r="F34" s="6">
+        <v>0</v>
+      </c>
+      <c r="G34" s="6">
+        <v>1</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J34" s="6">
+        <v>0</v>
+      </c>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>